<commit_message>
cambios en el certificado
</commit_message>
<xml_diff>
--- a/TempCal/CalibrationHistory.xlsx
+++ b/TempCal/CalibrationHistory.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>CALIBRATION DATE</t>
   </si>
@@ -47,37 +47,76 @@
     <t>RESULT</t>
   </si>
   <si>
+    <t>2016-11-08</t>
+  </si>
+  <si>
+    <t>FAHRENHEIT</t>
+  </si>
+  <si>
+    <t>HL</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>20.3</t>
+  </si>
+  <si>
+    <t>60.5</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>207.23508</t>
+  </si>
+  <si>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>PROCESS PASSED</t>
+  </si>
+  <si>
+    <t>2016-11-24</t>
+  </si>
+  <si>
+    <t>CELSIUS</t>
+  </si>
+  <si>
+    <t>60.3</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>74.850006</t>
+  </si>
+  <si>
+    <t>60.1</t>
+  </si>
+  <si>
+    <t>PROCESS FAILED</t>
+  </si>
+  <si>
     <t>2016-11-22</t>
   </si>
   <si>
-    <t>CELSIUS</t>
-  </si>
-  <si>
-    <t>SDF</t>
-  </si>
-  <si>
-    <t>213123</t>
-  </si>
-  <si>
-    <t>12.1</t>
-  </si>
-  <si>
-    <t>50.1</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>76.33658</t>
-  </si>
-  <si>
-    <t>15.1</t>
-  </si>
-  <si>
-    <t>15.3</t>
-  </si>
-  <si>
-    <t>PROCESS PASSED</t>
+    <t>DFD</t>
+  </si>
+  <si>
+    <t>12313</t>
+  </si>
+  <si>
+    <t>70.1</t>
+  </si>
+  <si>
+    <t>69.9598</t>
+  </si>
+  <si>
+    <t>30.1</t>
+  </si>
+  <si>
+    <t>30.4</t>
   </si>
 </sst>
 </file>
@@ -192,10 +231,80 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>